<commit_message>
Adjusted time trends for retirement and education processes -cleaned up a bit `getDoubleValue()` of Person.java
</commit_message>
<xml_diff>
--- a/input/PL/parameters.xlsx
+++ b/input/PL/parameters.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10817"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10201"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pineapple/IdeaProjects/SimPathsEU/input/PL/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pineapple/IdeaProjects/SimPathsEU_JAN/input/PL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DDEF42F-C866-F94C-8401-B36BF785083C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{468A27D1-6BDB-7E4F-92C4-2A4F66811887}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="24900" yWindow="2780" windowWidth="20300" windowHeight="19580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="89">
   <si>
     <t>KEY</t>
   </si>
@@ -285,6 +285,9 @@
   </si>
   <si>
     <t>year of EM income data used in KeyFunctionHU2</t>
+  </si>
+  <si>
+    <t>MAX_AGE_TO_STAY_IN_CONTINUOUS_EDUCATION</t>
   </si>
 </sst>
 </file>
@@ -292,7 +295,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -369,7 +372,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -674,10 +677,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B41"/>
+  <dimension ref="A1:B40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -744,7 +747,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>88</v>
       </c>
       <c r="B8">
         <v>29</v>
@@ -752,143 +755,143 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B9">
-        <v>35</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B10">
-        <v>50</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B11">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B12">
-        <v>65</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B13">
-        <v>16</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B14">
-        <v>75</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B15">
-        <v>0.25</v>
+        <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B16">
-        <v>1.4999999999999999E-2</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B17">
-        <v>25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18">
-        <v>0</v>
+        <v>19</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>25</v>
+        <v>20</v>
+      </c>
+      <c r="B19">
+        <v>150</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B20">
-        <v>150</v>
+        <v>112</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B21">
-        <v>112</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22">
-        <v>0.5</v>
+      <c r="A22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="1">
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B23" s="1">
-        <v>6</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B24" s="1">
-        <v>2011</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B25" s="1">
-        <v>2020</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B26" s="1">
         <v>2019</v>
@@ -896,121 +899,113 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B27" s="1">
-        <v>2019</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B28" s="1">
-        <v>0</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B29" s="1">
-        <v>4000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B30" s="1">
-        <v>0</v>
+        <v>15000</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B31" s="1">
-        <v>15000</v>
+        <v>14</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B32" s="1">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B33" s="1">
-        <v>18</v>
+        <v>44</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B34" s="1">
-        <v>44</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B35" s="1">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B36" s="1">
         <v>0.5</v>
       </c>
     </row>
+    <row r="36" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B36" s="2">
+        <v>5.6000000000000001E-2</v>
+      </c>
+    </row>
     <row r="37" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A37" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B37" s="2">
-        <v>5.6000000000000001E-2</v>
+      <c r="A37" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B37" s="10">
+        <v>276</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="9" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B38" s="10">
-        <v>276</v>
+        <v>139</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="B39" s="10">
-        <v>139</v>
+        <v>82</v>
+      </c>
+      <c r="B39" s="9">
+        <v>45</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="9" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B40" s="9">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A41" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="B41" s="9">
         <v>2018</v>
       </c>
     </row>

</xml_diff>